<commit_message>
Expand class Dataframe - append column into existed xlsx; Complete B-F5.1
</commit_message>
<xml_diff>
--- a/test-data/F5_F6_NF1.xlsx
+++ b/test-data/F5_F6_NF1.xlsx
@@ -1,36 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ST 221\project3\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2AFF75-AEA7-412B-AEEC-8DECE90C063D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225F499C-5ADE-43E7-B15D-C013F4C1DDA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11369" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A-F2" sheetId="1" r:id="rId1"/>
     <sheet name="B-F5.1" sheetId="2" r:id="rId2"/>
-    <sheet name="B-F5.2" sheetId="4" r:id="rId3"/>
-    <sheet name="B-F5.3" sheetId="5" r:id="rId4"/>
-    <sheet name="B-F6" sheetId="6" r:id="rId5"/>
-    <sheet name="B-NF1" sheetId="7" r:id="rId6"/>
+    <sheet name="B-F5.2" sheetId="3" r:id="rId3"/>
+    <sheet name="B-F5.3" sheetId="4" r:id="rId4"/>
+    <sheet name="B-F6" sheetId="5" r:id="rId5"/>
+    <sheet name="B-NF1" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="123">
   <si>
     <t>ID</t>
   </si>
@@ -71,6 +67,9 @@
     <t>test5@example</t>
   </si>
   <si>
+    <t>0648793214</t>
+  </si>
+  <si>
     <t>123abc</t>
   </si>
   <si>
@@ -80,117 +79,159 @@
     <t>SU-003</t>
   </si>
   <si>
+    <t>mhung</t>
+  </si>
+  <si>
     <t>SU-004</t>
   </si>
   <si>
+    <t>r</t>
+  </si>
+  <si>
     <t>SU-005</t>
   </si>
   <si>
+    <t>yasommer2</t>
+  </si>
+  <si>
+    <t>test5.example</t>
+  </si>
+  <si>
     <t>SU-006</t>
   </si>
   <si>
+    <t>test5.example@</t>
+  </si>
+  <si>
     <t>SU-007</t>
   </si>
   <si>
+    <t>@</t>
+  </si>
+  <si>
     <t>SU-008</t>
   </si>
   <si>
+    <t>test5@example.</t>
+  </si>
+  <si>
     <t>SU-009</t>
   </si>
   <si>
+    <t>0648793ab4</t>
+  </si>
+  <si>
     <t>SU-010</t>
   </si>
   <si>
+    <t>12</t>
+  </si>
+  <si>
     <t>SU-011</t>
   </si>
   <si>
     <t>SU-012</t>
   </si>
   <si>
-    <t>mhung</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>test5.example</t>
-  </si>
-  <si>
-    <t>test5.example@</t>
-  </si>
-  <si>
-    <t>@</t>
-  </si>
-  <si>
-    <t>test5@example.</t>
-  </si>
-  <si>
-    <t>0648793214</t>
-  </si>
-  <si>
-    <t>0648793ab4</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>12aabc</t>
   </si>
   <si>
+    <t>Tên</t>
+  </si>
+  <si>
+    <t>Ngày</t>
+  </si>
+  <si>
+    <t>Mô tả</t>
+  </si>
+  <si>
+    <t>Địa chỉ</t>
+  </si>
+  <si>
+    <t>Thời lượng</t>
+  </si>
+  <si>
+    <t>Lặp lại</t>
+  </si>
+  <si>
+    <t>Tới</t>
+  </si>
+  <si>
+    <t>Tính bằng phút</t>
+  </si>
+  <si>
     <t>AE-01-001</t>
   </si>
   <si>
-    <t>Tên</t>
-  </si>
-  <si>
-    <t>Ngày</t>
-  </si>
-  <si>
-    <t>Mô tả</t>
-  </si>
-  <si>
-    <t>Địa chỉ</t>
-  </si>
-  <si>
-    <t>Thời lượng</t>
-  </si>
-  <si>
-    <t>Lặp lại</t>
-  </si>
-  <si>
-    <t>Tới</t>
+    <t>15/06/1975 11:59</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>fail</t>
   </si>
   <si>
     <t>AE-01-002</t>
   </si>
   <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>success</t>
+  </si>
+  <si>
     <t>AE-01-003</t>
   </si>
   <si>
+    <t>test event</t>
+  </si>
+  <si>
+    <t>01/01/1900 00:00</t>
+  </si>
+  <si>
     <t>AE-01-004</t>
   </si>
   <si>
+    <t>01/01/1900 00:01</t>
+  </si>
+  <si>
     <t>AE-01-005</t>
   </si>
   <si>
     <t>AE-01-006</t>
   </si>
   <si>
+    <t>31/12/2050 23:58</t>
+  </si>
+  <si>
     <t>AE-01-007</t>
   </si>
   <si>
+    <t>31/12/2050 23:59</t>
+  </si>
+  <si>
     <t>AE-01-008</t>
   </si>
   <si>
     <t>AE-01-009</t>
   </si>
   <si>
+    <t>D</t>
+  </si>
+  <si>
     <t>AE-01-010</t>
   </si>
   <si>
     <t>AE-01-011</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
     <t>AE-01-012</t>
   </si>
   <si>
@@ -227,54 +268,24 @@
     <t>AE-01-023</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>test event</t>
-  </si>
-  <si>
-    <t>15/06/1975 11:59</t>
-  </si>
-  <si>
-    <t>01/01/1900 00:00</t>
-  </si>
-  <si>
-    <t>01/01/1900 00:01</t>
-  </si>
-  <si>
-    <t>31/12/2050 23:58</t>
-  </si>
-  <si>
-    <t>31/12/2050 23:59</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
     <t>Không</t>
   </si>
   <si>
+    <t>Chọn</t>
+  </si>
+  <si>
+    <t>AE-02-001</t>
+  </si>
+  <si>
+    <t>A new event</t>
+  </si>
+  <si>
+    <t>24/12/2022 00:00</t>
+  </si>
+  <si>
     <t>x</t>
   </si>
   <si>
-    <t>Chọn</t>
-  </si>
-  <si>
-    <t>yasommer2</t>
-  </si>
-  <si>
-    <t>AE-02-001</t>
-  </si>
-  <si>
     <t>AE-02-002</t>
   </si>
   <si>
@@ -293,42 +304,36 @@
     <t>AE-02-007</t>
   </si>
   <si>
+    <t>15</t>
+  </si>
+  <si>
     <t>AE-02-008</t>
   </si>
   <si>
+    <t>4a</t>
+  </si>
+  <si>
     <t>AE-02-009</t>
   </si>
   <si>
     <t>AE-02-010</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>AE-02-011</t>
   </si>
   <si>
-    <t>A new event</t>
-  </si>
-  <si>
-    <t>24/12/2022 00:00</t>
-  </si>
-  <si>
-    <t>Tính bằng phút</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>4a</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>3r</t>
   </si>
   <si>
     <t>AE-03-001</t>
   </si>
   <si>
+    <t>test add a event</t>
+  </si>
+  <si>
     <t>AE-03-002</t>
   </si>
   <si>
@@ -347,9 +352,6 @@
     <t>AE-03-007</t>
   </si>
   <si>
-    <t>test add a event</t>
-  </si>
-  <si>
     <t>1d</t>
   </si>
   <si>
@@ -362,44 +364,44 @@
     <t>RE-001</t>
   </si>
   <si>
+    <t>T</t>
+  </si>
+  <si>
     <t>RE-002</t>
   </si>
   <si>
+    <t>O</t>
+  </si>
+  <si>
     <t>RE-003</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
-    <t>O</t>
+    <t>remove 1 or all?</t>
   </si>
   <si>
     <t>NFRE-001</t>
   </si>
   <si>
+    <t>All</t>
+  </si>
+  <si>
     <t>NFRE-002</t>
   </si>
   <si>
+    <t>One</t>
+  </si>
+  <si>
     <t>NFRE-003</t>
-  </si>
-  <si>
-    <t>remove 1 or all?</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>One</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,12 +421,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -456,7 +452,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -466,7 +462,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -475,10 +471,8 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -770,7 +764,8 @@
   <cols>
     <col min="1" max="1" width="7.296875" style="2" customWidth="1"/>
     <col min="2" max="8" width="15.69921875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.796875" style="2"/>
+    <col min="9" max="9" width="8.796875" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -816,18 +811,18 @@
         <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
@@ -839,21 +834,21 @@
         <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>10</v>
@@ -865,21 +860,21 @@
         <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
@@ -891,21 +886,21 @@
         <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>10</v>
@@ -914,24 +909,24 @@
         <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>10</v>
@@ -940,24 +935,24 @@
         <v>11</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>10</v>
@@ -966,24 +961,24 @@
         <v>11</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
@@ -992,24 +987,24 @@
         <v>11</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>10</v>
@@ -1021,21 +1016,21 @@
         <v>12</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>10</v>
@@ -1047,21 +1042,21 @@
         <v>12</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>10</v>
@@ -1073,21 +1068,21 @@
         <v>12</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>10</v>
@@ -1099,52 +1094,52 @@
         <v>12</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{7AB84B61-0319-4AA9-99E2-F03CFE816DDF}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{B802E67D-9167-46D7-A820-65E4990D4358}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{19CE3590-91F0-4996-A439-670A9D8FF826}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{08D79101-17BB-490D-8B68-9C07946D3D5A}"/>
-    <hyperlink ref="E6" r:id="rId5" display="test5@example" xr:uid="{F04937D0-4DD5-4D36-AB89-FD24DEFE0E5C}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{B7A496AE-6162-4BA6-B26F-769A04BB2F31}"/>
-    <hyperlink ref="E8" r:id="rId7" display="test5.example@" xr:uid="{CBB5BE51-6932-4119-88EE-9284F04B8FF4}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{0C69A07B-19FE-4FED-8BAF-C166A94F4FE6}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{55A964B1-B5D7-4F00-92E6-F61953B3E3BF}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{6B846F16-B7DA-4436-AE93-BBCC7FC18073}"/>
-    <hyperlink ref="E12" r:id="rId11" xr:uid="{DB4BEAFE-A278-4967-BB86-82AF05C491FF}"/>
-    <hyperlink ref="E13" r:id="rId12" xr:uid="{AC8DBE6A-AB65-4BF5-8B44-490234B128DF}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E6" r:id="rId5" display="test5@example" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E8" r:id="rId7" display="test5.example@" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84318381-EEF7-4616-BD09-CABEA10BEC9C}">
-  <dimension ref="A1:I25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="6" width="15.69921875" style="2" customWidth="1"/>
-    <col min="7" max="8" width="15.69921875" style="8" customWidth="1"/>
-    <col min="9" max="16384" width="8.796875" style="2"/>
+    <col min="7" max="8" width="15.69921875" customWidth="1"/>
+    <col min="9" max="9" width="8.796875" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1163,13 +1158,13 @@
       <c r="F1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="6" t="s">
         <v>41</v>
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1178,441 +1173,510 @@
       <c r="F2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="H2" s="9"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="I13" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="B18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="B21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="H21">
+        <v>4999999999</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" s="8">
+      <c r="C22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H22">
+        <v>9999999998</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23">
+        <v>9999999999</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G20" s="8">
+      <c r="I24" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H21" s="8">
-        <v>4999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H22" s="8">
-        <v>9999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H23" s="8">
-        <v>9999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H24" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H25" s="8">
-        <v>1</v>
+      <c r="I25" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:G1"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7D2CB9F-3316-4EC3-BEF9-99CA9D8F5C1D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1622,7 +1686,8 @@
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="10" width="15.69921875" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.796875" style="2"/>
+    <col min="11" max="11" width="8.796875" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1644,12 +1709,12 @@
       <c r="F1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
       <c r="I1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="7"/>
+      <c r="J1" s="9"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1659,203 +1724,203 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>42</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="G7" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="I9" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1863,13 +1928,12 @@
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:J1"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A36C4DF8-F856-48D1-8B70-D5A91527CFCA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1879,7 +1943,8 @@
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="10" width="15.69921875" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.796875" style="2"/>
+    <col min="11" max="11" width="8.796875" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1901,12 +1966,12 @@
       <c r="F1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
       <c r="I1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="7"/>
+      <c r="J1" s="9"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1916,135 +1981,135 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>42</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="I8" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2052,13 +2117,12 @@
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:J1"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{540BA5B8-2610-485F-BE1A-FBE894E8A693}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2075,26 +2139,26 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
         <v>112</v>
@@ -2105,24 +2169,23 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
         <v>114</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F34F8DBC-B8AA-4762-BBEE-E5D9EA2D8D52}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2139,15 +2202,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
         <v>112</v>
@@ -2158,29 +2221,63 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="B3" t="s">
         <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="J2:R3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="10:18" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" t="s">
+        <v>47</v>
+      </c>
+      <c r="R2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="10:18" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Complete B-F5.2 and B-F5.3
</commit_message>
<xml_diff>
--- a/test-data/F5_F6_NF1.xlsx
+++ b/test-data/F5_F6_NF1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ST 221\project3\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2208BF6-831B-4B25-BE1E-EC53B5F4DC38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BC2324-5D3A-4AC3-8286-02848D60974C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11369" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11369" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A-F2" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,13 @@
     <sheet name="B-F5.3" sheetId="4" r:id="rId4"/>
     <sheet name="B-F6" sheetId="5" r:id="rId5"/>
     <sheet name="B-NF1" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="125">
   <si>
     <t>ID</t>
   </si>
@@ -154,6 +153,9 @@
     <t>Lặp lại</t>
   </si>
   <si>
+    <t>Expect</t>
+  </si>
+  <si>
     <t>Tới</t>
   </si>
   <si>
@@ -268,12 +270,6 @@
     <t>AE-01-023</t>
   </si>
   <si>
-    <t>Không</t>
-  </si>
-  <si>
-    <t>Chọn</t>
-  </si>
-  <si>
     <t>AE-02-001</t>
   </si>
   <si>
@@ -283,63 +279,72 @@
     <t>24/12/2022 00:00</t>
   </si>
   <si>
+    <t>AE-02-002</t>
+  </si>
+  <si>
+    <t>AE-02-003</t>
+  </si>
+  <si>
+    <t>AE-02-004</t>
+  </si>
+  <si>
+    <t>AE-02-005</t>
+  </si>
+  <si>
+    <t>AE-02-006</t>
+  </si>
+  <si>
+    <t>&lt;null&gt;</t>
+  </si>
+  <si>
+    <t>AE-02-007</t>
+  </si>
+  <si>
+    <t>AE-02-008</t>
+  </si>
+  <si>
+    <t>f4r6</t>
+  </si>
+  <si>
+    <t>AE-02-009</t>
+  </si>
+  <si>
+    <t>AE-02-010</t>
+  </si>
+  <si>
+    <t>AE-02-011</t>
+  </si>
+  <si>
+    <t>3r</t>
+  </si>
+  <si>
+    <t>Go to another month</t>
+  </si>
+  <si>
+    <t>Open form</t>
+  </si>
+  <si>
+    <t>AE-03-001</t>
+  </si>
+  <si>
+    <t>button</t>
+  </si>
+  <si>
+    <t>test add a event</t>
+  </si>
+  <si>
+    <t>AE-03-002</t>
+  </si>
+  <si>
     <t>x</t>
   </si>
   <si>
-    <t>AE-02-002</t>
-  </si>
-  <si>
-    <t>AE-02-003</t>
-  </si>
-  <si>
-    <t>AE-02-004</t>
-  </si>
-  <si>
-    <t>AE-02-005</t>
-  </si>
-  <si>
-    <t>AE-02-006</t>
-  </si>
-  <si>
-    <t>AE-02-007</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>AE-02-008</t>
-  </si>
-  <si>
-    <t>4a</t>
-  </si>
-  <si>
-    <t>AE-02-009</t>
-  </si>
-  <si>
-    <t>AE-02-010</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>AE-02-011</t>
-  </si>
-  <si>
-    <t>3r</t>
-  </si>
-  <si>
-    <t>AE-03-001</t>
-  </si>
-  <si>
-    <t>test add a event</t>
-  </si>
-  <si>
-    <t>AE-03-002</t>
-  </si>
-  <si>
     <t>AE-03-003</t>
   </si>
   <si>
+    <t>cell</t>
+  </si>
+  <si>
     <t>AE-03-004</t>
   </si>
   <si>
@@ -352,7 +357,7 @@
     <t>AE-03-007</t>
   </si>
   <si>
-    <t>1d</t>
+    <t>d12</t>
   </si>
   <si>
     <t>isLoop?</t>
@@ -764,8 +769,8 @@
   <cols>
     <col min="1" max="1" width="7.296875" style="2" customWidth="1"/>
     <col min="2" max="8" width="15.69921875" style="2" customWidth="1"/>
-    <col min="9" max="12" width="8.796875" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="8.796875" style="2"/>
+    <col min="9" max="19" width="8.796875" style="2" customWidth="1"/>
+    <col min="20" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -1127,16 +1132,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="6" width="15.69921875" style="2" customWidth="1"/>
     <col min="7" max="8" width="15.69921875" customWidth="1"/>
-    <col min="9" max="12" width="8.796875" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="8.796875" style="2"/>
+    <col min="9" max="19" width="8.796875" style="2" customWidth="1"/>
+    <col min="20" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -1162,7 +1167,10 @@
       <c r="H1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
@@ -1171,499 +1179,498 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3"/>
+        <v>49</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="I16" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H21">
         <v>4999999999</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H22">
         <v>9999999998</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H23">
         <v>9999999999</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H25">
         <v>1</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1677,20 +1684,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="F1" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="10" width="15.69921875" style="2" customWidth="1"/>
-    <col min="11" max="14" width="8.796875" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="8.796875" style="2"/>
+    <col min="1" max="8" width="15.69921875" style="2" customWidth="1"/>
+    <col min="9" max="19" width="8.796875" style="2" customWidth="1"/>
+    <col min="20" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1710,223 +1717,209 @@
         <v>40</v>
       </c>
       <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="J2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="I3" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="F7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="I8" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="G9">
+        <v>15</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="G10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="H11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B13" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>99</v>
+      <c r="I13" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="I1:J1"/>
+  <mergeCells count="1">
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1934,188 +1927,206 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8:O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="10" width="15.69921875" style="2" customWidth="1"/>
-    <col min="11" max="14" width="8.796875" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="8.796875" style="2"/>
+    <col min="11" max="21" width="8.796875" style="2" customWidth="1"/>
+    <col min="22" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="9"/>
+      <c r="J1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
       <c r="H2" s="4" t="s">
         <v>43</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8">
+        <v>15</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B9" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>108</v>
+      <c r="E9" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>85</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="I1:J1"/>
+  <mergeCells count="1">
+    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2139,43 +2150,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" t="s">
         <v>116</v>
-      </c>
-      <c r="C4" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2202,82 +2213,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="J2:R3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="2" spans="10:18" x14ac:dyDescent="0.3">
-      <c r="J2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L2" t="s">
-        <v>45</v>
-      </c>
-      <c r="M2" t="s">
-        <v>46</v>
-      </c>
-      <c r="N2" t="s">
-        <v>47</v>
-      </c>
-      <c r="R2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="10:18" x14ac:dyDescent="0.3">
-      <c r="J3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
complete A-F2 and B-F6
</commit_message>
<xml_diff>
--- a/test-data/F5_F6_NF1.xlsx
+++ b/test-data/F5_F6_NF1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ST 221\project3\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42928644-CA2E-4981-8DC7-A89F5E887710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71414DD-6850-40FB-A49D-FB391E2B53D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11369" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2816" yWindow="2816" windowWidth="15474" windowHeight="8070" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A-F2" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="128">
   <si>
     <t>ID</t>
   </si>
@@ -360,6 +360,9 @@
     <t>d12</t>
   </si>
   <si>
+    <t>Event name</t>
+  </si>
+  <si>
     <t>isLoop?</t>
   </si>
   <si>
@@ -375,10 +378,16 @@
     <t>RE-002</t>
   </si>
   <si>
+    <t>b</t>
+  </si>
+  <si>
     <t>O</t>
   </si>
   <si>
     <t>RE-003</t>
+  </si>
+  <si>
+    <t>c</t>
   </si>
   <si>
     <t>F</t>
@@ -761,7 +770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2:J13"/>
     </sheetView>
   </sheetViews>
@@ -769,8 +778,8 @@
   <cols>
     <col min="1" max="1" width="7.296875" style="2" customWidth="1"/>
     <col min="2" max="8" width="15.69921875" style="2" customWidth="1"/>
-    <col min="9" max="24" width="8.796875" style="2" customWidth="1"/>
-    <col min="25" max="16384" width="8.796875" style="2"/>
+    <col min="9" max="32" width="8.796875" style="2" customWidth="1"/>
+    <col min="33" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -830,7 +839,9 @@
       <c r="I2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J2"/>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -857,7 +868,9 @@
       <c r="I3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J3"/>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -887,7 +900,9 @@
       <c r="I4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J4"/>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -917,7 +932,9 @@
       <c r="I5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J5"/>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -947,7 +964,9 @@
       <c r="I6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J6"/>
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -977,7 +996,9 @@
       <c r="I7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J7"/>
+      <c r="J7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -1007,7 +1028,9 @@
       <c r="I8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J8"/>
+      <c r="J8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -1037,7 +1060,9 @@
       <c r="I9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J9"/>
+      <c r="J9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -1067,7 +1092,9 @@
       <c r="I10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J10"/>
+      <c r="J10" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -1097,7 +1124,9 @@
       <c r="I11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J11"/>
+      <c r="J11" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -1127,7 +1156,9 @@
       <c r="I12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J12"/>
+      <c r="J12" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
@@ -1157,7 +1188,9 @@
       <c r="I13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J13"/>
+      <c r="J13" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1184,15 +1217,15 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="J3" sqref="J3:J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="6" width="15.69921875" style="2" customWidth="1"/>
     <col min="7" max="8" width="15.69921875" customWidth="1"/>
-    <col min="9" max="24" width="8.796875" style="2" customWidth="1"/>
-    <col min="25" max="16384" width="8.796875" style="2"/>
+    <col min="9" max="32" width="8.796875" style="2" customWidth="1"/>
+    <col min="33" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -1253,6 +1286,9 @@
       <c r="I3" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="J3" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -1273,6 +1309,9 @@
       <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="J4" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1293,6 +1332,9 @@
       <c r="I5" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="J5" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -1313,6 +1355,9 @@
       <c r="I6" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="J6" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -1333,6 +1378,9 @@
       <c r="I7" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="J7" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -1353,6 +1401,9 @@
       <c r="I8" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="J8" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -1373,6 +1424,9 @@
       <c r="I9" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="J9" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -1390,6 +1444,9 @@
       <c r="I10" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="J10" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -1410,6 +1467,9 @@
       <c r="I11" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="J11" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -1427,6 +1487,9 @@
       <c r="I12" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="J12" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
@@ -1447,6 +1510,9 @@
       <c r="I13" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="J13" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
@@ -1470,6 +1536,9 @@
       <c r="I14" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="J14" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
@@ -1493,6 +1562,9 @@
       <c r="I15" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="J15" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
@@ -1516,8 +1588,11 @@
       <c r="I16" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J16" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>72</v>
       </c>
@@ -1539,8 +1614,11 @@
       <c r="I17" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>73</v>
       </c>
@@ -1562,8 +1640,11 @@
       <c r="I18" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J18" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>74</v>
       </c>
@@ -1585,8 +1666,11 @@
       <c r="I19" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>75</v>
       </c>
@@ -1608,8 +1692,11 @@
       <c r="I20" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J20" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>76</v>
       </c>
@@ -1631,8 +1718,11 @@
       <c r="I21" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J21" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>77</v>
       </c>
@@ -1654,8 +1744,11 @@
       <c r="I22" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J22" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>78</v>
       </c>
@@ -1677,8 +1770,11 @@
       <c r="I23" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J23" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>79</v>
       </c>
@@ -1700,8 +1796,11 @@
       <c r="I24" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J24" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>80</v>
       </c>
@@ -1721,6 +1820,9 @@
         <v>1</v>
       </c>
       <c r="I25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1738,14 +1840,14 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G1"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="8" width="15.69921875" style="2" customWidth="1"/>
-    <col min="9" max="24" width="8.796875" style="2" customWidth="1"/>
-    <col min="25" max="16384" width="8.796875" style="2"/>
+    <col min="9" max="32" width="8.796875" style="2" customWidth="1"/>
+    <col min="33" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -1803,6 +1905,9 @@
       <c r="I3" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -1814,6 +1919,9 @@
       <c r="I4" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1831,6 +1939,9 @@
       <c r="I5" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -1848,6 +1959,9 @@
       <c r="I6" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="J6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -1865,6 +1979,9 @@
       <c r="I7" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -1882,6 +1999,9 @@
       <c r="I8" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="J8" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -1899,6 +2019,9 @@
       <c r="I9" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="J9" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -1916,6 +2039,9 @@
       <c r="I10" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="J10" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -1933,6 +2059,9 @@
       <c r="I11" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="J11" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -1950,6 +2079,9 @@
       <c r="I12" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="J12" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
@@ -1965,6 +2097,9 @@
         <v>96</v>
       </c>
       <c r="I13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1978,7 +2113,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="L8" sqref="L8:O9"/>
@@ -1987,11 +2122,11 @@
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="10" width="15.69921875" style="2" customWidth="1"/>
-    <col min="11" max="26" width="8.796875" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="8.796875" style="2"/>
+    <col min="11" max="34" width="8.796875" style="2" customWidth="1"/>
+    <col min="35" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2024,7 +2159,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -2039,7 +2174,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>99</v>
       </c>
@@ -2055,8 +2190,11 @@
       <c r="K3" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>102</v>
       </c>
@@ -2075,8 +2213,11 @@
       <c r="K4" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>104</v>
       </c>
@@ -2092,8 +2233,11 @@
       <c r="K5" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>106</v>
       </c>
@@ -2106,8 +2250,11 @@
       <c r="K6" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>107</v>
       </c>
@@ -2126,8 +2273,11 @@
       <c r="K7" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>108</v>
       </c>
@@ -2146,8 +2296,11 @@
       <c r="K8" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>109</v>
       </c>
@@ -2164,6 +2317,9 @@
         <v>110</v>
       </c>
       <c r="K9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2177,18 +2333,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="15.69921875" customWidth="1"/>
+    <col min="1" max="4" width="15.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2198,38 +2354,71 @@
       <c r="C1" s="6" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
         <v>115</v>
       </c>
-      <c r="B3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" t="s">
         <v>118</v>
       </c>
-      <c r="C4" t="s">
-        <v>116</v>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2243,7 +2432,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2256,43 +2445,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>